<commit_message>
Added missing shot location info
</commit_message>
<xml_diff>
--- a/source/excel/2016-olympic-qualifiers-concacaf/2016-olympic-qualifiers-concacaf-usa-pur-021516.xlsx
+++ b/source/excel/2016-olympic-qualifiers-concacaf/2016-olympic-qualifiers-concacaf-usa-pur-021516.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="3820" windowWidth="17700" windowHeight="21760" tabRatio="697"/>
+    <workbookView xWindow="-580" yWindow="300" windowWidth="25960" windowHeight="15140" tabRatio="697"/>
   </bookViews>
   <sheets>
     <sheet name="match" sheetId="1" r:id="rId1"/>
@@ -1866,9 +1866,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane ySplit="29" topLeftCell="A1430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1443" sqref="S1443"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane ySplit="29" topLeftCell="A1231" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1238" sqref="I1238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -51070,7 +51070,7 @@
         <v>50</v>
       </c>
       <c r="G807" s="30" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="H807" s="30" t="s">
         <v>20</v>
@@ -55798,7 +55798,7 @@
         <v>59</v>
       </c>
       <c r="G885" s="30" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="H885" s="30" t="s">
         <v>20</v>
@@ -66780,7 +66780,7 @@
         <v>50</v>
       </c>
       <c r="G1065" s="30" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H1065" s="30" t="s">
         <v>20</v>

</xml_diff>